<commit_message>
Complete report for sprint 6
</commit_message>
<xml_diff>
--- a/sprint-backlog/sprint-6/report-sheet.xlsx
+++ b/sprint-backlog/sprint-6/report-sheet.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffc\Git\Team14\sprint-backlog\sprint-6\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3227946F-11FF-4F4D-8DAA-41457F7B3643}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="986"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="report-sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="plan" sheetId="1" r:id="rId1"/>
     <sheet name="execution" sheetId="2" r:id="rId2"/>
     <sheet name="burndown" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -133,7 +139,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -250,14 +256,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-CA"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -299,12 +308,11 @@
                 </a:uFill>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Sprint 4: Burndown Chart Provisional vs Actual</a:t>
+              <a:t>Sprint 6: Burndown Chart Provisional vs Actual</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -332,6 +340,7 @@
               <a:solidFill>
                 <a:srgbClr val="636363"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
           </c:spPr>
@@ -366,6 +375,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9425-4846-BC7E-357C8AF2DBAB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -420,6 +434,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9425-4846-BC7E-357C8AF2DBAB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -436,7 +455,6 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="203401472"/>
         <c:axId val="203407360"/>
@@ -546,7 +564,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -605,7 +622,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -666,7 +689,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -699,9 +722,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -734,6 +774,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -909,18 +966,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="6" width="8.5546875"/>
-    <col min="7" max="7" width="10.44140625"/>
-    <col min="8" max="1025" width="8.5546875"/>
+    <col min="1" max="6" width="8.54296875"/>
+    <col min="7" max="7" width="10.453125"/>
+    <col min="8" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1111,16 +1168,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1025" width="8.5546875"/>
+    <col min="1" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1314,16 +1371,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1025" width="8.5546875"/>
+    <col min="1" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>